<commit_message>
make sure preview page work
</commit_message>
<xml_diff>
--- a/uploads/hi.xlsx
+++ b/uploads/hi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,62 +434,70 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Word</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Meaning</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hello</t>
+          <t>('Word', 'Hello')</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A greeting</t>
+          <t>('Meaning', 'A greeting')</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Goodbye</t>
+          <t>('Word', 'Goodbye')</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A farewell</t>
+          <t>('Meaning', 'A farewell')</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Thank you</t>
+          <t>('Word', 'Thank you')</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Gratitude</t>
+          <t>('Meaning', 'Gratitude')</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bonjour</t>
+          <t>('Word', 'bonjour')</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>dsf</t>
+          <t>('Meaning', 'dsf')</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('Word', 'hi')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>('Meaning', 'dfasf')</t>
         </is>
       </c>
     </row>

</xml_diff>